<commit_message>
sistemata altezza e larghezza celle che erano saltate, per facilitare la lettura
</commit_message>
<xml_diff>
--- a/Documents/RR/ExternalDocuments/AnalisiDeiRequisiti/requisiti/Requisiti_new.xlsx
+++ b/Documents/RR/ExternalDocuments/AnalisiDeiRequisiti/requisiti/Requisiti_new.xlsx
@@ -1,16 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Davide/Desktop/GitHub/Leaf/Documents/RR/ExternalDocuments/AnalisiDeiRequisiti/requisiti/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="700" yWindow="460" windowWidth="24900" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -779,11 +788,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -792,22 +798,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -815,7 +806,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -823,7 +814,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
+      <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -840,7 +831,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -848,103 +839,323 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="111" zoomScaleNormal="111" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B107" activeCellId="0" sqref="B107"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="111" zoomScalePageLayoutView="111" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="79.506976744186"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.6697674418605"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.506976744186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.6697674418605"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6651162790698"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="81.5" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -958,7 +1169,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -969,7 +1180,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -983,7 +1194,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -997,7 +1208,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +1222,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
@@ -1022,7 +1233,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1033,7 +1244,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -1047,7 +1258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1058,7 +1269,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -1069,7 +1280,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1080,7 +1291,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -1091,7 +1302,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -1102,7 +1313,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -1113,7 +1324,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1124,7 +1335,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>39</v>
       </c>
@@ -1135,7 +1346,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>26</v>
       </c>
@@ -1146,7 +1357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1157,7 +1368,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>44</v>
       </c>
@@ -1168,7 +1379,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>46</v>
       </c>
@@ -1179,7 +1390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>30</v>
       </c>
@@ -1190,7 +1401,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>32</v>
       </c>
@@ -1201,7 +1412,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>50</v>
       </c>
@@ -1212,7 +1423,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -1226,7 +1437,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>55</v>
       </c>
@@ -1238,7 +1449,7 @@
       </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>57</v>
       </c>
@@ -1249,7 +1460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>59</v>
       </c>
@@ -1260,7 +1471,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>61</v>
       </c>
@@ -1271,7 +1482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
@@ -1282,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>65</v>
       </c>
@@ -1294,7 +1505,7 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>67</v>
       </c>
@@ -1305,7 +1516,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>69</v>
       </c>
@@ -1316,7 +1527,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>71</v>
       </c>
@@ -1327,7 +1538,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>73</v>
       </c>
@@ -1338,7 +1549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>75</v>
       </c>
@@ -1349,7 +1560,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>77</v>
       </c>
@@ -1360,7 +1571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>79</v>
       </c>
@@ -1371,7 +1582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>81</v>
       </c>
@@ -1382,7 +1593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>83</v>
       </c>
@@ -1393,7 +1604,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>85</v>
       </c>
@@ -1407,7 +1618,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -1418,18 +1629,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" s="1" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
@@ -1443,7 +1654,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>91</v>
       </c>
@@ -1455,7 +1666,7 @@
       </c>
       <c r="D46" s="3"/>
     </row>
-    <row r="47" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>94</v>
       </c>
@@ -1467,7 +1678,7 @@
       </c>
       <c r="D47" s="3"/>
     </row>
-    <row r="48" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>97</v>
       </c>
@@ -1479,7 +1690,7 @@
       </c>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>100</v>
       </c>
@@ -1491,7 +1702,7 @@
       </c>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>103</v>
       </c>
@@ -1503,7 +1714,7 @@
       </c>
       <c r="D50" s="3"/>
     </row>
-    <row r="51" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>105</v>
       </c>
@@ -1515,7 +1726,7 @@
       </c>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>108</v>
       </c>
@@ -1527,7 +1738,7 @@
       </c>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>111</v>
       </c>
@@ -1539,7 +1750,7 @@
       </c>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" customFormat="false" ht="17" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="54" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>114</v>
       </c>
@@ -1553,7 +1764,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>118</v>
       </c>
@@ -1565,7 +1776,7 @@
       </c>
       <c r="D55" s="3"/>
     </row>
-    <row r="56" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>120</v>
       </c>
@@ -1577,7 +1788,7 @@
       </c>
       <c r="D56" s="3"/>
     </row>
-    <row r="57" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>122</v>
       </c>
@@ -1589,7 +1800,7 @@
       </c>
       <c r="D57" s="3"/>
     </row>
-    <row r="58" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>124</v>
       </c>
@@ -1601,7 +1812,7 @@
       </c>
       <c r="D58" s="3"/>
     </row>
-    <row r="59" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>126</v>
       </c>
@@ -1613,7 +1824,7 @@
       </c>
       <c r="D59" s="3"/>
     </row>
-    <row r="60" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>128</v>
       </c>
@@ -1625,7 +1836,7 @@
       </c>
       <c r="D60" s="3"/>
     </row>
-    <row r="61" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>131</v>
       </c>
@@ -1637,7 +1848,7 @@
       </c>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>134</v>
       </c>
@@ -1649,7 +1860,7 @@
       </c>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>137</v>
       </c>
@@ -1661,7 +1872,7 @@
       </c>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>140</v>
       </c>
@@ -1673,239 +1884,239 @@
       </c>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+    <row r="65" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
         <v>143</v>
       </c>
-      <c r="B65" s="0" t="s">
+      <c r="B65" t="s">
         <v>144</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" t="s">
         <v>145</v>
       </c>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
         <v>146</v>
       </c>
-      <c r="B66" s="0" t="s">
+      <c r="B66" t="s">
         <v>147</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" t="s">
         <v>148</v>
       </c>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="0" t="s">
+      <c r="B67" t="s">
         <v>150</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" t="s">
         <v>145</v>
       </c>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
         <v>151</v>
       </c>
-      <c r="B68" s="0" t="s">
+      <c r="B68" t="s">
         <v>152</v>
       </c>
-      <c r="C68" s="0" t="s">
+      <c r="C68" t="s">
         <v>148</v>
       </c>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
         <v>153</v>
       </c>
-      <c r="B69" s="0" t="s">
+      <c r="B69" t="s">
         <v>154</v>
       </c>
-      <c r="C69" s="0" t="s">
+      <c r="C69" t="s">
         <v>155</v>
       </c>
       <c r="D69" s="3"/>
     </row>
-    <row r="70" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
         <v>156</v>
       </c>
-      <c r="B70" s="0" t="s">
+      <c r="B70" t="s">
         <v>157</v>
       </c>
-      <c r="C70" s="0" t="s">
+      <c r="C70" t="s">
         <v>158</v>
       </c>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
         <v>159</v>
       </c>
-      <c r="B71" s="0" t="s">
+      <c r="B71" t="s">
         <v>160</v>
       </c>
-      <c r="C71" s="0" t="s">
+      <c r="C71" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
         <v>162</v>
       </c>
-      <c r="B72" s="0" t="s">
+      <c r="B72" t="s">
         <v>163</v>
       </c>
-      <c r="C72" s="0" t="s">
+      <c r="C72" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
         <v>165</v>
       </c>
-      <c r="B73" s="0" t="s">
+      <c r="B73" t="s">
         <v>166</v>
       </c>
-      <c r="C73" s="0" t="s">
+      <c r="C73" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
         <v>168</v>
       </c>
-      <c r="B74" s="0" t="s">
+      <c r="B74" t="s">
         <v>169</v>
       </c>
-      <c r="C74" s="0" t="s">
+      <c r="C74" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>171</v>
       </c>
-      <c r="B75" s="0" t="s">
+      <c r="B75" t="s">
         <v>172</v>
       </c>
-      <c r="C75" s="0" t="s">
+      <c r="C75" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
         <v>174</v>
       </c>
-      <c r="B76" s="0" t="s">
+      <c r="B76" t="s">
         <v>175</v>
       </c>
-      <c r="C76" s="0" t="s">
+      <c r="C76" t="s">
         <v>176</v>
       </c>
-      <c r="D76" s="0" t="s">
+      <c r="D76" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
         <v>178</v>
       </c>
-      <c r="B77" s="0" t="s">
+      <c r="B77" t="s">
         <v>179</v>
       </c>
-      <c r="C77" s="0" t="s">
+      <c r="C77" t="s">
         <v>180</v>
       </c>
-      <c r="D77" s="0" t="s">
+      <c r="D77" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
         <v>181</v>
       </c>
-      <c r="B78" s="0" t="s">
+      <c r="B78" t="s">
         <v>182</v>
       </c>
-      <c r="C78" s="0" t="s">
+      <c r="C78" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
         <v>184</v>
       </c>
-      <c r="B79" s="0" t="s">
+      <c r="B79" t="s">
         <v>185</v>
       </c>
-      <c r="D79" s="0" t="s">
+      <c r="D79" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
         <v>186</v>
       </c>
-      <c r="B80" s="0" t="s">
+      <c r="B80" t="s">
         <v>187</v>
       </c>
-      <c r="C80" s="0" t="s">
+      <c r="C80" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
         <v>189</v>
       </c>
-      <c r="B81" s="0" t="s">
+      <c r="B81" t="s">
         <v>190</v>
       </c>
-      <c r="C81" s="0" t="s">
+      <c r="C81" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
         <v>192</v>
       </c>
-      <c r="B82" s="0" t="s">
+      <c r="B82" t="s">
         <v>193</v>
       </c>
-      <c r="C82" s="0" t="s">
+      <c r="C82" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
         <v>195</v>
       </c>
-      <c r="B83" s="0" t="s">
+      <c r="B83" t="s">
         <v>196</v>
       </c>
-      <c r="C83" s="0" t="s">
+      <c r="C83" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
         <v>198</v>
       </c>
-      <c r="B84" s="0" t="s">
+      <c r="B84" t="s">
         <v>199</v>
       </c>
-      <c r="C84" s="0" t="s">
+      <c r="C84" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" s="7" t="s">
         <v>201</v>
       </c>
@@ -1917,7 +2128,7 @@
       </c>
       <c r="D85" s="7"/>
     </row>
-    <row r="86" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" s="7" t="s">
         <v>204</v>
       </c>
@@ -1929,7 +2140,7 @@
       </c>
       <c r="D86" s="7"/>
     </row>
-    <row r="87" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" s="7" t="s">
         <v>207</v>
       </c>
@@ -1943,7 +2154,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" s="7" t="s">
         <v>211</v>
       </c>
@@ -1955,7 +2166,7 @@
       </c>
       <c r="D88" s="7"/>
     </row>
-    <row r="89" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" s="7" t="s">
         <v>214</v>
       </c>
@@ -1967,7 +2178,7 @@
       </c>
       <c r="D89" s="7"/>
     </row>
-    <row r="90" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" s="7" t="s">
         <v>217</v>
       </c>
@@ -1979,7 +2190,7 @@
       </c>
       <c r="D90" s="7"/>
     </row>
-    <row r="91" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>220</v>
       </c>
@@ -1991,7 +2202,7 @@
       </c>
       <c r="D91" s="7"/>
     </row>
-    <row r="92" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>222</v>
       </c>
@@ -2003,7 +2214,7 @@
       </c>
       <c r="D92" s="7"/>
     </row>
-    <row r="93" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" s="7" t="s">
         <v>224</v>
       </c>
@@ -2015,7 +2226,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" s="7" t="s">
         <v>227</v>
       </c>
@@ -2027,7 +2238,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" s="7" t="s">
         <v>229</v>
       </c>
@@ -2039,7 +2250,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" s="7" t="s">
         <v>231</v>
       </c>
@@ -2051,7 +2262,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" s="7" t="s">
         <v>233</v>
       </c>
@@ -2062,17 +2273,17 @@
         <v>226</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A98" s="7"/>
       <c r="B98" s="7"/>
       <c r="D98" s="7"/>
     </row>
-    <row r="99" s="1" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>1</v>
       </c>
@@ -2086,7 +2297,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="7" t="s">
         <v>236</v>
       </c>
@@ -2098,7 +2309,7 @@
       </c>
       <c r="D101" s="7"/>
     </row>
-    <row r="102" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="7" t="s">
         <v>238</v>
       </c>
@@ -2110,7 +2321,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="7" t="s">
         <v>241</v>
       </c>
@@ -2120,7 +2331,7 @@
       <c r="C103" s="7"/>
       <c r="D103" s="7"/>
     </row>
-    <row r="104" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="7" t="s">
         <v>243</v>
       </c>
@@ -2130,7 +2341,7 @@
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
     </row>
-    <row r="105" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="7" t="s">
         <v>245</v>
       </c>
@@ -2142,7 +2353,7 @@
       </c>
       <c r="D105" s="7"/>
     </row>
-    <row r="106" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="7" t="s">
         <v>247</v>
       </c>
@@ -2153,17 +2364,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="7"/>
       <c r="B107" s="7"/>
       <c r="D107" s="7"/>
     </row>
-    <row r="108" s="1" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="108" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="19" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="109" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>1</v>
       </c>
@@ -2177,7 +2388,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A110" s="7" t="s">
         <v>250</v>
       </c>
@@ -2191,17 +2402,12 @@
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="1:1"/>
-    <mergeCell ref="44:44"/>
-    <mergeCell ref="99:99"/>
-    <mergeCell ref="108:108"/>
+    <mergeCell ref="A1:XFD1"/>
+    <mergeCell ref="A44:XFD44"/>
+    <mergeCell ref="A99:XFD99"/>
+    <mergeCell ref="A108:XFD108"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
iniziato l'aggiornamento dei requisiti
</commit_message>
<xml_diff>
--- a/Documents/RR/ExternalDocuments/AnalisiDeiRequisiti/requisiti/Requisiti_new.xlsx
+++ b/Documents/RR/ExternalDocuments/AnalisiDeiRequisiti/requisiti/Requisiti_new.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="280">
   <si>
     <t>REQUISITI DI VINCOLO</t>
   </si>
@@ -62,9 +62,6 @@
     <t>RObbV2.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare lo scenario funzionale</t>
-  </si>
-  <si>
     <t>scenario individuato: navigazione</t>
   </si>
   <si>
@@ -80,15 +77,9 @@
     <t>RObbV2.3</t>
   </si>
   <si>
-    <t>Il gruppo deve scegliere i componenti HW</t>
-  </si>
-  <si>
     <t>RObbV2.4</t>
   </si>
   <si>
-    <t>Il gruppo deve scegliere i componenti SW</t>
-  </si>
-  <si>
     <t>RObbV2.5</t>
   </si>
   <si>
@@ -101,120 +92,54 @@
     <t>RObbV2.6</t>
   </si>
   <si>
-    <t>Il gruppo deve documentare le scelte relative al laboratorio</t>
-  </si>
-  <si>
     <t>RObbV3</t>
   </si>
   <si>
-    <t>Il gruppo deve sviluppare un prototipo SW (che operi) all'interno dell'area prevista</t>
-  </si>
-  <si>
     <t>RObbV3.1</t>
   </si>
   <si>
-    <t>Il prototipo si deve basare sui concetti di IPS e smart places</t>
-  </si>
-  <si>
     <t>RObbV3.2</t>
   </si>
   <si>
-    <t>Il SW sviluppato deve essere per smartphone</t>
-  </si>
-  <si>
-    <t>RObbV3.2.1</t>
-  </si>
-  <si>
-    <t>Il sistema operativo dello smartphone deve essere Android o iOS</t>
-  </si>
-  <si>
-    <t>ROpzV3.2.1.1</t>
-  </si>
-  <si>
     <t>Il gruppo deve sviluppare il prototipo sia per Android che per iOS</t>
   </si>
   <si>
-    <t>RObbV3.2.1.2</t>
-  </si>
-  <si>
-    <t>La versione del sistema operativo Android deve essere almeno la 5.0</t>
-  </si>
-  <si>
     <t>Riunione interna</t>
   </si>
   <si>
-    <t>ROpzV3.2.1.3</t>
-  </si>
-  <si>
-    <t>La versione del sistema operativo Android deve essere almeno la 4.4</t>
-  </si>
-  <si>
     <t>Riunione esterna</t>
   </si>
   <si>
     <t>RObbV4</t>
   </si>
   <si>
-    <t>Il gruppo deve effettuare una sperimentazione pratica del laboratorio e del prototipo</t>
-  </si>
-  <si>
     <t>RObbV4.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche HW</t>
-  </si>
-  <si>
     <t>RObbV4.1.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche HW lato apparecchio mobile</t>
-  </si>
-  <si>
     <t>RObbV4.1.2</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche HW lato beacon</t>
-  </si>
-  <si>
     <t>RObbV4.2</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche lato SW</t>
-  </si>
-  <si>
     <t>RObbV4.2.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche lato SW riguardo la navigazione</t>
-  </si>
-  <si>
-    <t>RObbV4.2.2</t>
-  </si>
-  <si>
-    <t>Il gruppo deve individuare le problematiche lato SW riguardo la comunicazione</t>
-  </si>
-  <si>
     <t>RObbV4.3</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare le problematiche lato UX</t>
-  </si>
-  <si>
     <t>UX = user experience</t>
   </si>
   <si>
     <t>RObbV4.3.1</t>
   </si>
   <si>
-    <t>Il gruppo deve presentare in modo intuitivo l'area coperta dalla funzionalità IPS</t>
-  </si>
-  <si>
     <t>RObbV4.3.2</t>
   </si>
   <si>
-    <t>L'applicazione deve proporre destinazioni o punti di interesse verso i quali viaggiare</t>
-  </si>
-  <si>
     <t>RObbV4.3.3</t>
   </si>
   <si>
@@ -227,54 +152,21 @@
     <t>Il gruppo deve eseguire almeno due sperimentazioni pratiche</t>
   </si>
   <si>
-    <t>RDesV4.5</t>
-  </si>
-  <si>
-    <t>Il gruppo deve simulare condizioni dell'ambiente il più possibili realistiche</t>
-  </si>
-  <si>
-    <t>RDesV4.5.1</t>
-  </si>
-  <si>
-    <t>Il gruppo deve simulare un numero congruo di persone rispetto all'ambiente scelto</t>
-  </si>
-  <si>
-    <t>RDesV4.5.2</t>
-  </si>
-  <si>
-    <t>Il gruppo deve simulare un numero di utilizzatori congruo all'ambiente scelto</t>
-  </si>
-  <si>
     <t>RObbV5</t>
   </si>
   <si>
-    <t>Il gruppo deve produrre e consegnare la documentazione dello studio</t>
-  </si>
-  <si>
     <t>RObbV5.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare e documentare alcune best practice</t>
-  </si>
-  <si>
     <t>RObbV5.1.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare e documentare alcune best practice per l'allestimento dell'impianto</t>
-  </si>
-  <si>
     <t>RObbV5.1.2</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare e documentare alcune best practice per il software</t>
-  </si>
-  <si>
     <t>RObbV5.1.3</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare e documentare alcune best practice per l'interazione con l'utente</t>
-  </si>
-  <si>
     <t>RObbV5.2</t>
   </si>
   <si>
@@ -290,39 +182,21 @@
     <t>RObbV5.2.2</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare un possibile scenario alternativo</t>
-  </si>
-  <si>
     <t>RObbV5.3</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare eventuali punti deboli della soluzione</t>
-  </si>
-  <si>
     <t>RObbV5.3.1</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare eventuali punti deboli HW della soluzione</t>
-  </si>
-  <si>
     <t>RObbV5.3.2</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare eventuali punti deboli SW della soluzione</t>
-  </si>
-  <si>
     <t>RObbV5.3.3</t>
   </si>
   <si>
-    <t>Il gruppo deve individuare eventuali punti deboli UX della soluzione</t>
-  </si>
-  <si>
     <t>RObbV5.4</t>
   </si>
   <si>
-    <t>Il gruppo deve consegnare la documentazione sulla mappa di distribuzione dei beacon</t>
-  </si>
-  <si>
     <t>REQUISITI FUNZIONALI</t>
   </si>
   <si>
@@ -840,6 +714,156 @@
   </si>
   <si>
     <t>L'applicazione deve fornire la possibilità di ricercare la destinazione tra quelle possibili all'interno dell'edificio</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare lo scenario funzionale da svikuppare</t>
+  </si>
+  <si>
+    <t>Il gruppo deve scegliere i componenti software</t>
+  </si>
+  <si>
+    <t>Il gruppo deve scegliere la tipologia di beacon tra quelli forniti</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare e motivare le scelte relative al laboratorio</t>
+  </si>
+  <si>
+    <t>Il gruppo deve sviluppare un prototipo software che operi all'interno dell'area indoor scelta</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche hardware</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche lato user experience</t>
+  </si>
+  <si>
+    <t>RObbV3.3</t>
+  </si>
+  <si>
+    <t>RObbV3.3.1</t>
+  </si>
+  <si>
+    <t>ROpzV3.3.1.1</t>
+  </si>
+  <si>
+    <t>RObbV3.3.1.2</t>
+  </si>
+  <si>
+    <t>ROpzV3.3.1.3</t>
+  </si>
+  <si>
+    <t>Il prototipo deve permettere di indicare la posizione, anche approssimativa, di un utente all'interno di un edificio (IPS)</t>
+  </si>
+  <si>
+    <t>Il prototipo deve permettere di fornire informazioni all'utente relative all'area mappata dal beacon (smart places)</t>
+  </si>
+  <si>
+    <t>Il software deve essere sviluppato per dispositivo mobile</t>
+  </si>
+  <si>
+    <t>Il sistema operativo del dispositivo mobile deve essere Android o iOS</t>
+  </si>
+  <si>
+    <t>La versione del sistema operativo Android deve essere compresa tra la versione 4.4 e la versione 5.1</t>
+  </si>
+  <si>
+    <t>La versione del sistema operativo Android deve essere superiore alla versione 4.4</t>
+  </si>
+  <si>
+    <t>Il gruppo deve effettuare una sperimentazione pratica del prototipo sulla base delle scelte fatte</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche hardware riguardanti l'apparecchio mobile</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche hardware riguardanti i beacon</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche software</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare le problematiche software riguardanti la navigazione</t>
+  </si>
+  <si>
+    <t>Il gruppo deve presentare in modo intuitivo l'area indoor scelta</t>
+  </si>
+  <si>
+    <t>L'applicazione deve proporre destinazioni verso le quali viaggiare</t>
+  </si>
+  <si>
+    <t>RObbV4.4.1</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare le scelte e le variazioni introdotte per ogni sperimentazione</t>
+  </si>
+  <si>
+    <t>RObbV4.5</t>
+  </si>
+  <si>
+    <t>Il gruppo deve simulare condizioni dell'ambiente il più possibili realistiche per quanto riguarda il numero di persone all'interno dell'area indoor scelta</t>
+  </si>
+  <si>
+    <t>Il gruppo deve produrre la documentazione dello studio</t>
+  </si>
+  <si>
+    <t>RObbV5.4.1</t>
+  </si>
+  <si>
+    <t>RObbV5.4.2</t>
+  </si>
+  <si>
+    <t>RObbV5.4.3</t>
+  </si>
+  <si>
+    <t>RObbV5.4.4</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione dell'impianto realizzato in varie versioni</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione della mappa di distribuzione degli apparecchi beacon</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione riguardante la densità dell'impianto</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione riguardante le scelte nel posizionamento dei beacon</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione riguardante le note operative dell'impianto</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare eventuali punti deboli della soluzione</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare eventuali punti deboli della soluzione riguardanti l'hardware</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare eventuali punti deboli della soluzione riguardanti il software</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare eventuali punti deboli della soluzione riguardanti l'user experience</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare e motivare le scelte fatte</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare e motivare le scelte fatte riguardo l'allestimento dell'impianto</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare e motivare le scelte fatte riguardo il software sviluppato</t>
+  </si>
+  <si>
+    <t>Il gruppo deve documentare e motivare le scelte fatte riguardo l'interazione con l'utente</t>
+  </si>
+  <si>
+    <t>RObbV5.5</t>
+  </si>
+  <si>
+    <t>Il gruppo deve realizzare la documentazione del percorso di ricerca e miglioramento</t>
+  </si>
+  <si>
+    <t>Il gruppo deve individuare un possibile scenario alternativo che eviti il verificarsi degli errori individuati</t>
   </si>
 </sst>
 </file>
@@ -899,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -914,6 +938,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1192,41 +1217,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
-      <selection activeCell="A100" sqref="A100:XFD100"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="125" zoomScaleNormal="95" zoomScalePageLayoutView="95" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="113.6640625" customWidth="1"/>
+    <col min="2" max="2" width="122.33203125" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
     <col min="4" max="4" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="7" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="6" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
@@ -1276,35 +1301,35 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>232</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>7</v>
@@ -1312,10 +1337,10 @@
     </row>
     <row r="13" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>231</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -1323,24 +1348,24 @@
     </row>
     <row r="14" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>25</v>
+        <v>233</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>7</v>
@@ -1348,10 +1373,10 @@
     </row>
     <row r="16" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>234</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -1359,21 +1384,21 @@
     </row>
     <row r="17" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>29</v>
+        <v>242</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>243</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>7</v>
@@ -1381,10 +1406,10 @@
     </row>
     <row r="19" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>32</v>
+        <v>237</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>33</v>
+        <v>244</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>7</v>
@@ -1392,10 +1417,10 @@
     </row>
     <row r="20" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>238</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>35</v>
+        <v>245</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>7</v>
@@ -1403,43 +1428,43 @@
     </row>
     <row r="21" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>239</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>39</v>
+        <v>240</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>40</v>
+        <v>246</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>241</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>43</v>
+        <v>247</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>45</v>
+        <v>248</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>7</v>
@@ -1447,10 +1472,10 @@
     </row>
     <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>235</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>7</v>
@@ -1458,10 +1483,10 @@
     </row>
     <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>49</v>
+        <v>249</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>7</v>
@@ -1469,10 +1494,10 @@
     </row>
     <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>250</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>7</v>
@@ -1480,10 +1505,10 @@
     </row>
     <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>251</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>7</v>
@@ -1491,10 +1516,10 @@
     </row>
     <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>55</v>
+        <v>252</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>7</v>
@@ -1502,24 +1527,24 @@
     </row>
     <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
+        <v>236</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>59</v>
+        <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>60</v>
+        <v>253</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>7</v>
@@ -1527,10 +1552,10 @@
     </row>
     <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>62</v>
+        <v>254</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>7</v>
@@ -1538,10 +1563,10 @@
     </row>
     <row r="33" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>7</v>
@@ -1549,21 +1574,21 @@
     </row>
     <row r="34" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>65</v>
+        <v>40</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>255</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>68</v>
+        <v>256</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>7</v>
@@ -1571,10 +1596,10 @@
     </row>
     <row r="36" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>69</v>
+        <v>257</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>70</v>
+        <v>258</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>7</v>
@@ -1582,10 +1607,10 @@
     </row>
     <row r="37" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>72</v>
+        <v>259</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>7</v>
@@ -1593,10 +1618,10 @@
     </row>
     <row r="38" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>74</v>
+        <v>273</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>7</v>
@@ -1604,10 +1629,10 @@
     </row>
     <row r="39" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>274</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>7</v>
@@ -1615,10 +1640,10 @@
     </row>
     <row r="40" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>275</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>7</v>
@@ -1626,10 +1651,10 @@
     </row>
     <row r="41" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>79</v>
+        <v>46</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>80</v>
+        <v>276</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>7</v>
@@ -1637,10 +1662,10 @@
     </row>
     <row r="42" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>7</v>
@@ -1648,10 +1673,10 @@
     </row>
     <row r="43" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
-        <v>83</v>
+        <v>49</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>84</v>
+        <v>50</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>7</v>
@@ -1659,10 +1684,10 @@
     </row>
     <row r="44" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
-        <v>85</v>
+        <v>51</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>86</v>
+        <v>279</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>7</v>
@@ -1670,21 +1695,22 @@
     </row>
     <row r="45" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>87</v>
+        <v>52</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>88</v>
+        <v>269</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>7</v>
       </c>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>89</v>
+        <v>53</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>90</v>
+        <v>270</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>7</v>
@@ -1693,10 +1719,10 @@
     </row>
     <row r="47" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>92</v>
+        <v>271</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>7</v>
@@ -1705,10 +1731,10 @@
     </row>
     <row r="48" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>93</v>
+        <v>55</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>94</v>
+        <v>272</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>7</v>
@@ -1717,819 +1743,861 @@
     </row>
     <row r="49" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>96</v>
+        <v>264</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="3"/>
-    </row>
-    <row r="50" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>97</v>
+        <v>260</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>98</v>
+        <v>265</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+    <row r="51" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="6" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D53" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D54" s="3"/>
-    </row>
-    <row r="55" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D55" s="3"/>
-    </row>
-    <row r="56" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" s="3"/>
-    </row>
-    <row r="57" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>111</v>
+        <v>58</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>107</v>
+        <v>60</v>
       </c>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>261</v>
+        <v>61</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>113</v>
+        <v>229</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>114</v>
+        <v>62</v>
       </c>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>115</v>
+        <v>63</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>118</v>
+        <v>66</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>119</v>
+        <v>67</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>120</v>
+        <v>68</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>121</v>
+        <v>69</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>122</v>
+        <v>70</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>124</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>125</v>
+        <v>219</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>126</v>
+        <v>71</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="D63" s="3"/>
     </row>
     <row r="64" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>127</v>
+        <v>73</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>128</v>
+        <v>74</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="D64" s="3"/>
     </row>
     <row r="65" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>129</v>
+        <v>76</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>131</v>
+        <v>79</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D66" s="3"/>
+        <v>81</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="67" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>123</v>
+        <v>81</v>
       </c>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>137</v>
+        <v>81</v>
       </c>
       <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>140</v>
+        <v>81</v>
       </c>
       <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>141</v>
+        <v>89</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>142</v>
+        <v>90</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>143</v>
+        <v>81</v>
       </c>
       <c r="D70" s="3"/>
     </row>
-    <row r="71" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>262</v>
+        <v>92</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>145</v>
+        <v>81</v>
       </c>
       <c r="D71" s="3"/>
     </row>
     <row r="72" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>146</v>
+        <v>93</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>147</v>
+        <v>94</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>148</v>
+        <v>95</v>
       </c>
       <c r="D72" s="3"/>
     </row>
     <row r="73" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>149</v>
-      </c>
-      <c r="B73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" t="s">
-        <v>151</v>
+      <c r="A73" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>98</v>
       </c>
       <c r="D73" s="3"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>152</v>
-      </c>
-      <c r="B74" t="s">
-        <v>153</v>
-      </c>
-      <c r="C74" t="s">
-        <v>154</v>
+    <row r="74" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="D74" s="3"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>155</v>
-      </c>
-      <c r="B75" t="s">
-        <v>156</v>
-      </c>
-      <c r="C75" t="s">
-        <v>151</v>
+    <row r="75" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="D75" s="3"/>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>157</v>
-      </c>
-      <c r="B76" t="s">
-        <v>158</v>
+    <row r="76" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="D76" s="3"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>159</v>
+        <v>107</v>
       </c>
       <c r="B77" t="s">
-        <v>160</v>
+        <v>108</v>
+      </c>
+      <c r="C77" t="s">
+        <v>109</v>
       </c>
       <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>161</v>
+        <v>110</v>
       </c>
       <c r="B78" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="C78" t="s">
-        <v>154</v>
+        <v>112</v>
       </c>
       <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="B79" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="C79" t="s">
-        <v>165</v>
+        <v>109</v>
       </c>
       <c r="D79" s="3"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="B80" t="s">
-        <v>167</v>
-      </c>
-      <c r="C80" t="s">
-        <v>168</v>
-      </c>
-      <c r="D80" s="4"/>
+        <v>116</v>
+      </c>
+      <c r="D80" s="3"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
-      </c>
-      <c r="C81" t="s">
-        <v>171</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
+        <v>120</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>175</v>
+        <v>121</v>
       </c>
       <c r="B83" t="s">
-        <v>176</v>
+        <v>122</v>
       </c>
       <c r="C83" t="s">
-        <v>177</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>178</v>
+        <v>124</v>
       </c>
       <c r="B84" t="s">
-        <v>179</v>
+        <v>125</v>
       </c>
       <c r="C84" t="s">
-        <v>180</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="B85" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
       <c r="C85" t="s">
-        <v>183</v>
+        <v>129</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>184</v>
+        <v>130</v>
       </c>
       <c r="B86" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="C86" t="s">
-        <v>186</v>
+        <v>132</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>187</v>
+        <v>133</v>
       </c>
       <c r="B87" t="s">
-        <v>265</v>
+        <v>134</v>
       </c>
       <c r="C87" t="s">
-        <v>188</v>
+        <v>135</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>189</v>
+        <v>136</v>
       </c>
       <c r="B88" t="s">
-        <v>190</v>
+        <v>137</v>
       </c>
       <c r="C88" t="s">
-        <v>191</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>192</v>
+        <v>139</v>
       </c>
       <c r="B89" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="C89" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="B90" t="s">
-        <v>195</v>
+        <v>143</v>
       </c>
       <c r="C90" t="s">
-        <v>196</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="B91" t="s">
-        <v>198</v>
+        <v>223</v>
       </c>
       <c r="C91" t="s">
-        <v>199</v>
+        <v>146</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>200</v>
+        <v>147</v>
       </c>
       <c r="B92" t="s">
-        <v>201</v>
+        <v>148</v>
       </c>
       <c r="C92" t="s">
-        <v>202</v>
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>203</v>
+        <v>150</v>
       </c>
       <c r="B93" t="s">
-        <v>204</v>
+        <v>151</v>
       </c>
       <c r="C93" t="s">
-        <v>205</v>
+        <v>81</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>206</v>
+        <v>152</v>
       </c>
       <c r="B94" t="s">
-        <v>207</v>
+        <v>153</v>
       </c>
       <c r="C94" t="s">
-        <v>208</v>
+        <v>154</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>209</v>
-      </c>
-      <c r="B95" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D95" s="5"/>
+        <v>155</v>
+      </c>
+      <c r="B95" t="s">
+        <v>156</v>
+      </c>
+      <c r="C95" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="B96" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="D96" s="5"/>
+      <c r="A96" t="s">
+        <v>158</v>
+      </c>
+      <c r="B96" t="s">
+        <v>159</v>
+      </c>
+      <c r="C96" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B97" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="C97" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="D97" s="5" t="s">
-        <v>218</v>
+      <c r="A97" t="s">
+        <v>161</v>
+      </c>
+      <c r="B97" t="s">
+        <v>162</v>
+      </c>
+      <c r="C97" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="B98" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C98" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D98" s="5"/>
+      <c r="A98" t="s">
+        <v>164</v>
+      </c>
+      <c r="B98" t="s">
+        <v>165</v>
+      </c>
+      <c r="C98" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="5" t="s">
-        <v>222</v>
+      <c r="A99" t="s">
+        <v>167</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>223</v>
+        <v>168</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>224</v>
+        <v>169</v>
       </c>
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A100" s="5" t="s">
-        <v>225</v>
+        <v>170</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>226</v>
+        <v>171</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>227</v>
+        <v>172</v>
       </c>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A101" s="5" t="s">
-        <v>228</v>
+        <v>173</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>229</v>
+        <v>174</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="D101" s="5"/>
+        <v>175</v>
+      </c>
+      <c r="D101" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A102" s="5" t="s">
-        <v>230</v>
+        <v>177</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>227</v>
+        <v>179</v>
       </c>
       <c r="D102" s="5"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A103" s="5" t="s">
-        <v>232</v>
+        <v>180</v>
       </c>
       <c r="B103" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5" t="s">
-        <v>234</v>
-      </c>
+        <v>181</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A104" s="5" t="s">
-        <v>235</v>
+        <v>183</v>
       </c>
       <c r="B104" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5" t="s">
-        <v>234</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C104" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A105" s="5" t="s">
-        <v>237</v>
+        <v>186</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C105" s="5"/>
-      <c r="D105" s="5" t="s">
-        <v>234</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A106" s="5" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5" t="s">
-        <v>234</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A107" s="5" t="s">
-        <v>241</v>
+        <v>190</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>242</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="C107" s="5"/>
       <c r="D107" s="5" t="s">
-        <v>234</v>
+        <v>192</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A108" s="5"/>
-      <c r="B108" s="5"/>
-      <c r="D108" s="5"/>
-    </row>
-    <row r="109" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D110" s="2" t="s">
-        <v>4</v>
+      <c r="A108" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A111" s="5" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C111" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D111" s="5"/>
+        <v>200</v>
+      </c>
+      <c r="D111" s="5" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A112" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A113" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="B113" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="5"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A114" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="B114" s="5" t="s">
-        <v>252</v>
-      </c>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="A112" s="5"/>
+      <c r="B112" s="5"/>
+      <c r="D112" s="5"/>
+    </row>
+    <row r="113" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A113" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A114" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A115" s="5" t="s">
-        <v>253</v>
+        <v>202</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>254</v>
+        <v>203</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>38</v>
+        <v>182</v>
       </c>
       <c r="D115" s="5"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A116" s="5" t="s">
-        <v>255</v>
+        <v>204</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>256</v>
-      </c>
-      <c r="C116" s="5" t="s">
-        <v>38</v>
+        <v>205</v>
+      </c>
+      <c r="C116" s="5"/>
+      <c r="D116" s="5" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A117" s="5"/>
-      <c r="B117" s="5"/>
+      <c r="A117" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C117" s="5"/>
       <c r="D117" s="5"/>
     </row>
-    <row r="118" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A119" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D119" s="2" t="s">
-        <v>4</v>
-      </c>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C118" s="5"/>
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B119" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D119" s="5"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A120" s="5" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="B120" s="5" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>260</v>
-      </c>
-      <c r="D120" s="5"/>
+        <v>26</v>
+      </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A121" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="B121" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C121" t="s">
-        <v>270</v>
+      <c r="A121" s="5"/>
+      <c r="B121" s="5"/>
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" spans="1:4" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="A122" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A123" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B124" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D124" s="5"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B125" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="C125" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>